<commit_message>
updated according to predict sets
</commit_message>
<xml_diff>
--- a/battlesim-parser/predict-table.xlsx
+++ b/battlesim-parser/predict-table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marius\Documents\UNI\P4-code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marius\Documents\UNI\P4-code\battlesim-parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -589,7 +589,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -610,13 +610,25 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -628,10 +640,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -642,45 +655,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Ugyldig" xfId="1" builtinId="27"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -801,6 +782,40 @@
       </font>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -815,16 +830,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel2" displayName="Tabel2" ref="B2:H121" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabel2" displayName="Tabel2" ref="B2:H121" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="B2:H121"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="Rule" dataDxfId="8"/>
-    <tableColumn id="2" name="Nonterminal" dataDxfId="7"/>
-    <tableColumn id="3" name="Productions" dataDxfId="6"/>
-    <tableColumn id="4" name="First set" dataDxfId="5"/>
-    <tableColumn id="5" name="Derives Empty?" dataDxfId="4"/>
-    <tableColumn id="6" name="Follow set" dataDxfId="3"/>
-    <tableColumn id="7" name="Kolonne1" dataDxfId="2"/>
+    <tableColumn id="1" name="Rule" dataDxfId="6"/>
+    <tableColumn id="2" name="Nonterminal" dataDxfId="5"/>
+    <tableColumn id="3" name="Productions" dataDxfId="4"/>
+    <tableColumn id="4" name="First set" dataDxfId="3"/>
+    <tableColumn id="5" name="Derives Empty?" dataDxfId="2"/>
+    <tableColumn id="6" name="Follow set" dataDxfId="1"/>
+    <tableColumn id="7" name="Kolonne1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1095,8 +1110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="B27" sqref="A27:XFD27"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E115" sqref="E115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1471,7 +1486,7 @@
       <c r="D21" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="6" t="s">
         <v>142</v>
       </c>
       <c r="F21" s="3" t="s">
@@ -1488,7 +1503,7 @@
       <c r="D22" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E22" s="6" t="s">
         <v>142</v>
       </c>
       <c r="F22" s="3" t="s">
@@ -1505,7 +1520,7 @@
       <c r="D23" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="6" t="s">
         <v>142</v>
       </c>
       <c r="F23" s="3" t="s">
@@ -1522,7 +1537,7 @@
       <c r="D24" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="6" t="s">
         <v>142</v>
       </c>
       <c r="F24" s="3" t="s">
@@ -1717,7 +1732,7 @@
       <c r="D35" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="6" t="s">
         <v>117</v>
       </c>
       <c r="F35" s="3" t="s">
@@ -1734,7 +1749,7 @@
       <c r="D36" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="E36" s="3" t="s">
+      <c r="E36" s="6" t="s">
         <v>117</v>
       </c>
       <c r="F36" s="3" t="s">
@@ -1751,7 +1766,7 @@
       <c r="D37" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="6" t="s">
         <v>117</v>
       </c>
       <c r="F37" s="3" t="s">
@@ -1806,7 +1821,7 @@
       <c r="D40" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="E40" s="6" t="s">
         <v>144</v>
       </c>
       <c r="F40" s="3" t="s">
@@ -1823,7 +1838,7 @@
       <c r="D41" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="6" t="s">
         <v>144</v>
       </c>
       <c r="F41" s="3" t="s">
@@ -2217,7 +2232,7 @@
       <c r="D63" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E63" s="6" t="s">
         <v>162</v>
       </c>
       <c r="F63" s="3" t="s">
@@ -2234,7 +2249,7 @@
       <c r="D64" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="E64" s="6" t="s">
         <v>156</v>
       </c>
       <c r="F64" s="3" t="s">
@@ -2251,7 +2266,7 @@
       <c r="D65" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E65" s="3" t="s">
+      <c r="E65" s="6" t="s">
         <v>71</v>
       </c>
       <c r="F65" s="3" t="s">
@@ -2270,7 +2285,7 @@
       <c r="D66" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="E66" s="6" t="s">
         <v>71</v>
       </c>
       <c r="F66" s="3" t="s">
@@ -2287,7 +2302,7 @@
       <c r="D67" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="E67" s="6" t="s">
         <v>71</v>
       </c>
       <c r="F67" s="3" t="s">
@@ -2306,7 +2321,7 @@
       <c r="D68" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="E68" s="6" t="s">
         <v>156</v>
       </c>
       <c r="F68" s="3" t="s">
@@ -2323,7 +2338,7 @@
       <c r="D69" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E69" s="3" t="s">
+      <c r="E69" s="6" t="s">
         <v>162</v>
       </c>
       <c r="F69" s="3" t="s">
@@ -2340,7 +2355,7 @@
       <c r="D70" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E70" s="3" t="s">
+      <c r="E70" s="6" t="s">
         <v>156</v>
       </c>
       <c r="F70" s="3" t="s">
@@ -2357,7 +2372,7 @@
       <c r="D71" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="E71" s="3" t="s">
+      <c r="E71" s="6" t="s">
         <v>162</v>
       </c>
       <c r="F71" s="3" t="s">
@@ -2980,7 +2995,7 @@
       <c r="D106" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E106" s="3" t="s">
+      <c r="E106" s="6" t="s">
         <v>71</v>
       </c>
       <c r="F106" s="3" t="s">
@@ -3065,7 +3080,7 @@
       <c r="D111" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="E111" s="3" t="s">
+      <c r="E111" s="6" t="s">
         <v>168</v>
       </c>
       <c r="F111" s="3" t="s">

</xml_diff>